<commit_message>
update certificate admin page
</commit_message>
<xml_diff>
--- a/public/asset/pdf/admin/university/exampleExcelList.xlsx
+++ b/public/asset/pdf/admin/university/exampleExcelList.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pulse\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\BELTEI-website\public\asset\pdf\admin\university\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C0A1B63-8868-4774-BE8C-45708411C9C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95283FE0-2E5E-4179-AAB1-A0A557D36BB5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2FF20A8B-344F-47C7-94F4-D6FF610DCBA8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{2FF20A8B-344F-47C7-94F4-D6FF610DCBA8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1914" uniqueCount="962">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2002" uniqueCount="1050">
   <si>
     <t>student id</t>
   </si>
@@ -2912,6 +2913,270 @@
   </si>
   <si>
     <t>HENG SEYHA</t>
+  </si>
+  <si>
+    <t>Major</t>
+  </si>
+  <si>
+    <t>Faculty</t>
+  </si>
+  <si>
+    <t>Major name in English</t>
+  </si>
+  <si>
+    <t>Major name in Khmer</t>
+  </si>
+  <si>
+    <t>General Management</t>
+  </si>
+  <si>
+    <t>គ្រប់គ្រងទូទៅ</t>
+  </si>
+  <si>
+    <t>International Business</t>
+  </si>
+  <si>
+    <t>ពាណិជ្ជកម្មអន្ដរជាតិ</t>
+  </si>
+  <si>
+    <t>Entrepreneurship and Innovation</t>
+  </si>
+  <si>
+    <t>សហគ្រិន និងនវានុវត្តន៌</t>
+  </si>
+  <si>
+    <t>Accounting</t>
+  </si>
+  <si>
+    <t>គណនេយ្យ</t>
+  </si>
+  <si>
+    <t>Marketing</t>
+  </si>
+  <si>
+    <t>ទីផ្សារ</t>
+  </si>
+  <si>
+    <t>Finance and Banking</t>
+  </si>
+  <si>
+    <t>ហិរញ្ញវត្ថុ និងធនាគារ</t>
+  </si>
+  <si>
+    <t>International Banking</t>
+  </si>
+  <si>
+    <t>ធនាគារអន្ដរជាតិ</t>
+  </si>
+  <si>
+    <t>Financial Technology</t>
+  </si>
+  <si>
+    <t>បច្ចេកវិទ្យាហិរញ្ញវត្ថុ</t>
+  </si>
+  <si>
+    <t>Economic</t>
+  </si>
+  <si>
+    <t>សេដ្ឋកិច្ច</t>
+  </si>
+  <si>
+    <t>Development Economic</t>
+  </si>
+  <si>
+    <t>អភិវឌ្ឍន៌សេដ្ឋកិច្ច</t>
+  </si>
+  <si>
+    <t>International Economic</t>
+  </si>
+  <si>
+    <t>សេដ្ឋកិច្ចអន្ដរជាតិ</t>
+  </si>
+  <si>
+    <t>Digital Economy</t>
+  </si>
+  <si>
+    <t>សេដ្ឋកិច្ចឌីជីថល</t>
+  </si>
+  <si>
+    <t>Law</t>
+  </si>
+  <si>
+    <t>ច្បាប់</t>
+  </si>
+  <si>
+    <t>Private Law</t>
+  </si>
+  <si>
+    <t>ច្បាប់ឯកជន</t>
+  </si>
+  <si>
+    <t>International Law</t>
+  </si>
+  <si>
+    <t>ច្បាប់អន្ដរជាតិ</t>
+  </si>
+  <si>
+    <t>Public Administration</t>
+  </si>
+  <si>
+    <t>រដ្ឋាបាលសាធារណៈ</t>
+  </si>
+  <si>
+    <t>Education Administrantion and Leadership</t>
+  </si>
+  <si>
+    <t>រដ្ឋបាលអប់រំ និងភាពជាអ្នកដឹកនាំ</t>
+  </si>
+  <si>
+    <t>Teaching English as a Foreign Language</t>
+  </si>
+  <si>
+    <t>បង្រៀនភាសាអង់គ្លេស</t>
+  </si>
+  <si>
+    <t>Communication Education</t>
+  </si>
+  <si>
+    <t>សាគមនាគមន៌អប់រំ</t>
+  </si>
+  <si>
+    <t>Khmer Literature</t>
+  </si>
+  <si>
+    <t>អក្សរសាស្រ្ដខ្មែរ</t>
+  </si>
+  <si>
+    <t>Mathematics</t>
+  </si>
+  <si>
+    <t>គណិតវិទ្យា</t>
+  </si>
+  <si>
+    <t>Physics</t>
+  </si>
+  <si>
+    <t>រូបវិទ្យា</t>
+  </si>
+  <si>
+    <t>Chemistry</t>
+  </si>
+  <si>
+    <t>គីមីវិទ្យា</t>
+  </si>
+  <si>
+    <t>Tourism Management</t>
+  </si>
+  <si>
+    <t>គ្រប់គ្រងទេសចរណ៌</t>
+  </si>
+  <si>
+    <t>Hotel Management</t>
+  </si>
+  <si>
+    <t>គ្រប់គ្រងសណ្ឋាគារ</t>
+  </si>
+  <si>
+    <t>Hospitality Management</t>
+  </si>
+  <si>
+    <t>គ្រប់គ្រងបដិសណ្ឋាកិច្ច</t>
+  </si>
+  <si>
+    <t>Software Engineering</t>
+  </si>
+  <si>
+    <t>វិស្វកម្មសហ្វវែ</t>
+  </si>
+  <si>
+    <t>Computer Networking and Cyber Security</t>
+  </si>
+  <si>
+    <t>បណ្ដាញកុំព្យូទ័រ និងសុវត្តិភាពបច្ចេកវិទ្យាព័ត៏មានវិទ្យា</t>
+  </si>
+  <si>
+    <t>Computer Graphic Design</t>
+  </si>
+  <si>
+    <t>រចនាពហុប្រព័ន្ធផ្សផ្សាយ</t>
+  </si>
+  <si>
+    <t>Digital Technology</t>
+  </si>
+  <si>
+    <t>បច្ចេកវិទ្យាឌិជីថល</t>
+  </si>
+  <si>
+    <t>Digital Communication and Media</t>
+  </si>
+  <si>
+    <t>ទំនាក់ទំនងឌីជីថល និងប្រព័ន្ធផ្សផ្សាយ</t>
+  </si>
+  <si>
+    <t>Eletronic and Telecommunication Engineering</t>
+  </si>
+  <si>
+    <t>វិស្វកម្មអេឡិត្រូនិច​ និងទូរគមនាគមន៌</t>
+  </si>
+  <si>
+    <t>Civil Engineering</t>
+  </si>
+  <si>
+    <t>វិស្វកម្មសំណង់ស៊ីវិល</t>
+  </si>
+  <si>
+    <t>Construction Engineering and Management</t>
+  </si>
+  <si>
+    <t>គ្រប់គ្រងវិស្វកម្មសំណង់</t>
+  </si>
+  <si>
+    <t>Architecture and Urbanization</t>
+  </si>
+  <si>
+    <t>ស្ថាបត្យកម្ម និងនគរូបនីយកម្ម</t>
+  </si>
+  <si>
+    <t>Interior Design</t>
+  </si>
+  <si>
+    <t>ស្ថាបត្យកម្មអគារ</t>
+  </si>
+  <si>
+    <t>International Relation</t>
+  </si>
+  <si>
+    <t>ទំនាក់ទំនងអន្ដរជាតិ</t>
+  </si>
+  <si>
+    <t>Diplomacy</t>
+  </si>
+  <si>
+    <t>ការទូត</t>
+  </si>
+  <si>
+    <t>International Affairs and Negotiations</t>
+  </si>
+  <si>
+    <t>កិច្ចការអន្ដរជាតិ និងការចរចា</t>
+  </si>
+  <si>
+    <t>Airline and Airport Management</t>
+  </si>
+  <si>
+    <t>គ្រប់គ្រងក្រុមហ៊ុនអាកាសចរន៌</t>
+  </si>
+  <si>
+    <t>Aviation Management</t>
+  </si>
+  <si>
+    <t>គ្រប់គ្រងវិស័យអាកាសចរណ៌</t>
+  </si>
+  <si>
+    <t>Aircraft Maintenance Engineering</t>
+  </si>
+  <si>
+    <t>វិស្វកម្មថែទាំយន្ដហោះ</t>
   </si>
 </sst>
 </file>
@@ -2921,7 +3186,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3025,8 +3290,21 @@
       <family val="1"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="!Khmer OS Siemreap"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3042,6 +3320,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3122,7 +3412,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3213,6 +3503,24 @@
     </xf>
     <xf numFmtId="15" fontId="8" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3531,7 +3839,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33793CBC-9267-45DA-9B1C-DF8BFDAB4A83}">
   <dimension ref="A1:J478"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
@@ -17407,4 +17715,627 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C911A01-FC32-4C84-A9CA-1DB9B8195DE8}">
+  <dimension ref="A1:D43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="31" t="s">
+        <v>962</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>963</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>964</v>
+      </c>
+      <c r="D1" s="31" t="s">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="23.25" x14ac:dyDescent="0.65">
+      <c r="A2" s="32">
+        <v>1</v>
+      </c>
+      <c r="B2" s="33">
+        <v>1</v>
+      </c>
+      <c r="C2" s="34" t="s">
+        <v>966</v>
+      </c>
+      <c r="D2" s="35" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="23.25" x14ac:dyDescent="0.65">
+      <c r="A3" s="32">
+        <v>2</v>
+      </c>
+      <c r="B3" s="33">
+        <v>1</v>
+      </c>
+      <c r="C3" s="34" t="s">
+        <v>968</v>
+      </c>
+      <c r="D3" s="35" t="s">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="23.25" x14ac:dyDescent="0.65">
+      <c r="A4" s="32">
+        <v>3</v>
+      </c>
+      <c r="B4" s="33">
+        <v>1</v>
+      </c>
+      <c r="C4" s="34" t="s">
+        <v>970</v>
+      </c>
+      <c r="D4" s="35" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="23.25" x14ac:dyDescent="0.65">
+      <c r="A5" s="32">
+        <v>4</v>
+      </c>
+      <c r="B5" s="33">
+        <v>1</v>
+      </c>
+      <c r="C5" s="34" t="s">
+        <v>972</v>
+      </c>
+      <c r="D5" s="35" t="s">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="23.25" x14ac:dyDescent="0.65">
+      <c r="A6" s="32">
+        <v>5</v>
+      </c>
+      <c r="B6" s="33">
+        <v>1</v>
+      </c>
+      <c r="C6" s="34" t="s">
+        <v>974</v>
+      </c>
+      <c r="D6" s="35" t="s">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="23.25" x14ac:dyDescent="0.65">
+      <c r="A7" s="32">
+        <v>6</v>
+      </c>
+      <c r="B7" s="33">
+        <v>2</v>
+      </c>
+      <c r="C7" s="34" t="s">
+        <v>976</v>
+      </c>
+      <c r="D7" s="35" t="s">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="23.25" x14ac:dyDescent="0.65">
+      <c r="A8" s="32">
+        <v>7</v>
+      </c>
+      <c r="B8" s="33">
+        <v>2</v>
+      </c>
+      <c r="C8" s="34" t="s">
+        <v>978</v>
+      </c>
+      <c r="D8" s="35" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="23.25" x14ac:dyDescent="0.65">
+      <c r="A9" s="32">
+        <v>8</v>
+      </c>
+      <c r="B9" s="33">
+        <v>2</v>
+      </c>
+      <c r="C9" s="34" t="s">
+        <v>980</v>
+      </c>
+      <c r="D9" s="35" t="s">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="23.25" x14ac:dyDescent="0.65">
+      <c r="A10" s="32">
+        <v>9</v>
+      </c>
+      <c r="B10" s="33">
+        <v>3</v>
+      </c>
+      <c r="C10" s="34" t="s">
+        <v>982</v>
+      </c>
+      <c r="D10" s="35" t="s">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="23.25" x14ac:dyDescent="0.65">
+      <c r="A11" s="32">
+        <v>10</v>
+      </c>
+      <c r="B11" s="33">
+        <v>3</v>
+      </c>
+      <c r="C11" s="34" t="s">
+        <v>984</v>
+      </c>
+      <c r="D11" s="35" t="s">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="23.25" x14ac:dyDescent="0.65">
+      <c r="A12" s="32">
+        <v>11</v>
+      </c>
+      <c r="B12" s="33">
+        <v>3</v>
+      </c>
+      <c r="C12" s="34" t="s">
+        <v>986</v>
+      </c>
+      <c r="D12" s="35" t="s">
+        <v>987</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="23.25" x14ac:dyDescent="0.65">
+      <c r="A13" s="32">
+        <v>12</v>
+      </c>
+      <c r="B13" s="33">
+        <v>3</v>
+      </c>
+      <c r="C13" s="34" t="s">
+        <v>988</v>
+      </c>
+      <c r="D13" s="35" t="s">
+        <v>989</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="23.25" x14ac:dyDescent="0.65">
+      <c r="A14" s="32">
+        <v>13</v>
+      </c>
+      <c r="B14" s="33">
+        <v>4</v>
+      </c>
+      <c r="C14" s="34" t="s">
+        <v>990</v>
+      </c>
+      <c r="D14" s="35" t="s">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="23.25" x14ac:dyDescent="0.65">
+      <c r="A15" s="32">
+        <v>14</v>
+      </c>
+      <c r="B15" s="33">
+        <v>4</v>
+      </c>
+      <c r="C15" s="34" t="s">
+        <v>992</v>
+      </c>
+      <c r="D15" s="35" t="s">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="23.25" x14ac:dyDescent="0.65">
+      <c r="A16" s="32">
+        <v>15</v>
+      </c>
+      <c r="B16" s="33">
+        <v>4</v>
+      </c>
+      <c r="C16" s="34" t="s">
+        <v>994</v>
+      </c>
+      <c r="D16" s="35" t="s">
+        <v>995</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="23.25" x14ac:dyDescent="0.65">
+      <c r="A17" s="32">
+        <v>16</v>
+      </c>
+      <c r="B17" s="33">
+        <v>4</v>
+      </c>
+      <c r="C17" s="34" t="s">
+        <v>996</v>
+      </c>
+      <c r="D17" s="35" t="s">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="23.25" x14ac:dyDescent="0.65">
+      <c r="A18" s="32">
+        <v>17</v>
+      </c>
+      <c r="B18" s="33">
+        <v>5</v>
+      </c>
+      <c r="C18" s="34" t="s">
+        <v>998</v>
+      </c>
+      <c r="D18" s="35" t="s">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="23.25" x14ac:dyDescent="0.65">
+      <c r="A19" s="32">
+        <v>18</v>
+      </c>
+      <c r="B19" s="33">
+        <v>5</v>
+      </c>
+      <c r="C19" s="34" t="s">
+        <v>1000</v>
+      </c>
+      <c r="D19" s="35" t="s">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="23.25" x14ac:dyDescent="0.65">
+      <c r="A20" s="32">
+        <v>19</v>
+      </c>
+      <c r="B20" s="33">
+        <v>5</v>
+      </c>
+      <c r="C20" s="34" t="s">
+        <v>1002</v>
+      </c>
+      <c r="D20" s="35" t="s">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="23.25" x14ac:dyDescent="0.65">
+      <c r="A21" s="32">
+        <v>20</v>
+      </c>
+      <c r="B21" s="33">
+        <v>5</v>
+      </c>
+      <c r="C21" s="34" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D21" s="35" t="s">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="23.25" x14ac:dyDescent="0.65">
+      <c r="A22" s="32">
+        <v>21</v>
+      </c>
+      <c r="B22" s="33">
+        <v>5</v>
+      </c>
+      <c r="C22" s="34" t="s">
+        <v>1006</v>
+      </c>
+      <c r="D22" s="35" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="23.25" x14ac:dyDescent="0.65">
+      <c r="A23" s="32">
+        <v>22</v>
+      </c>
+      <c r="B23" s="33">
+        <v>5</v>
+      </c>
+      <c r="C23" s="34" t="s">
+        <v>1008</v>
+      </c>
+      <c r="D23" s="35" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="23.25" x14ac:dyDescent="0.65">
+      <c r="A24" s="32">
+        <v>23</v>
+      </c>
+      <c r="B24" s="33">
+        <v>5</v>
+      </c>
+      <c r="C24" s="34" t="s">
+        <v>1010</v>
+      </c>
+      <c r="D24" s="35" t="s">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="23.25" x14ac:dyDescent="0.65">
+      <c r="A25" s="32">
+        <v>24</v>
+      </c>
+      <c r="B25" s="33">
+        <v>6</v>
+      </c>
+      <c r="C25" s="34" t="s">
+        <v>1012</v>
+      </c>
+      <c r="D25" s="35" t="s">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="23.25" x14ac:dyDescent="0.65">
+      <c r="A26" s="32">
+        <v>25</v>
+      </c>
+      <c r="B26" s="33">
+        <v>6</v>
+      </c>
+      <c r="C26" s="34" t="s">
+        <v>1014</v>
+      </c>
+      <c r="D26" s="35" t="s">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="23.25" x14ac:dyDescent="0.65">
+      <c r="A27" s="32">
+        <v>26</v>
+      </c>
+      <c r="B27" s="33">
+        <v>6</v>
+      </c>
+      <c r="C27" s="34" t="s">
+        <v>1016</v>
+      </c>
+      <c r="D27" s="35" t="s">
+        <v>1017</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="23.25" x14ac:dyDescent="0.65">
+      <c r="A28" s="32">
+        <v>27</v>
+      </c>
+      <c r="B28" s="33">
+        <v>7</v>
+      </c>
+      <c r="C28" s="34" t="s">
+        <v>1018</v>
+      </c>
+      <c r="D28" s="35" t="s">
+        <v>1019</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="23.25" x14ac:dyDescent="0.65">
+      <c r="A29" s="32">
+        <v>28</v>
+      </c>
+      <c r="B29" s="33">
+        <v>7</v>
+      </c>
+      <c r="C29" s="34" t="s">
+        <v>1020</v>
+      </c>
+      <c r="D29" s="35" t="s">
+        <v>1021</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="23.25" x14ac:dyDescent="0.65">
+      <c r="A30" s="32">
+        <v>29</v>
+      </c>
+      <c r="B30" s="33">
+        <v>7</v>
+      </c>
+      <c r="C30" s="34" t="s">
+        <v>1022</v>
+      </c>
+      <c r="D30" s="35" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="23.25" x14ac:dyDescent="0.65">
+      <c r="A31" s="32">
+        <v>30</v>
+      </c>
+      <c r="B31" s="33">
+        <v>8</v>
+      </c>
+      <c r="C31" s="34" t="s">
+        <v>1024</v>
+      </c>
+      <c r="D31" s="35" t="s">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="23.25" x14ac:dyDescent="0.65">
+      <c r="A32" s="32">
+        <v>31</v>
+      </c>
+      <c r="B32" s="33">
+        <v>8</v>
+      </c>
+      <c r="C32" s="34" t="s">
+        <v>1026</v>
+      </c>
+      <c r="D32" s="35" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="23.25" x14ac:dyDescent="0.65">
+      <c r="A33" s="32">
+        <v>32</v>
+      </c>
+      <c r="B33" s="33">
+        <v>8</v>
+      </c>
+      <c r="C33" s="34" t="s">
+        <v>1028</v>
+      </c>
+      <c r="D33" s="35" t="s">
+        <v>1029</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="23.25" x14ac:dyDescent="0.65">
+      <c r="A34" s="32">
+        <v>33</v>
+      </c>
+      <c r="B34" s="33">
+        <v>9</v>
+      </c>
+      <c r="C34" s="34" t="s">
+        <v>1030</v>
+      </c>
+      <c r="D34" s="35" t="s">
+        <v>1031</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="23.25" x14ac:dyDescent="0.65">
+      <c r="A35" s="32">
+        <v>34</v>
+      </c>
+      <c r="B35" s="33">
+        <v>9</v>
+      </c>
+      <c r="C35" s="34" t="s">
+        <v>1032</v>
+      </c>
+      <c r="D35" s="35" t="s">
+        <v>1033</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="23.25" x14ac:dyDescent="0.65">
+      <c r="A36" s="32">
+        <v>35</v>
+      </c>
+      <c r="B36" s="33">
+        <v>10</v>
+      </c>
+      <c r="C36" s="34" t="s">
+        <v>1034</v>
+      </c>
+      <c r="D36" s="35" t="s">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="23.25" x14ac:dyDescent="0.65">
+      <c r="A37" s="32">
+        <v>36</v>
+      </c>
+      <c r="B37" s="33">
+        <v>10</v>
+      </c>
+      <c r="C37" s="34" t="s">
+        <v>1036</v>
+      </c>
+      <c r="D37" s="35" t="s">
+        <v>1037</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="23.25" x14ac:dyDescent="0.65">
+      <c r="A38" s="32">
+        <v>37</v>
+      </c>
+      <c r="B38" s="33">
+        <v>11</v>
+      </c>
+      <c r="C38" s="34" t="s">
+        <v>1038</v>
+      </c>
+      <c r="D38" s="35" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="23.25" x14ac:dyDescent="0.65">
+      <c r="A39" s="32">
+        <v>38</v>
+      </c>
+      <c r="B39" s="33">
+        <v>11</v>
+      </c>
+      <c r="C39" s="34" t="s">
+        <v>1040</v>
+      </c>
+      <c r="D39" s="35" t="s">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="23.25" x14ac:dyDescent="0.65">
+      <c r="A40" s="32">
+        <v>39</v>
+      </c>
+      <c r="B40" s="33">
+        <v>11</v>
+      </c>
+      <c r="C40" s="34" t="s">
+        <v>1042</v>
+      </c>
+      <c r="D40" s="35" t="s">
+        <v>1043</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="23.25" x14ac:dyDescent="0.65">
+      <c r="A41" s="32">
+        <v>40</v>
+      </c>
+      <c r="B41" s="33">
+        <v>12</v>
+      </c>
+      <c r="C41" s="34" t="s">
+        <v>1044</v>
+      </c>
+      <c r="D41" s="35" t="s">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="23.25" x14ac:dyDescent="0.65">
+      <c r="A42" s="32">
+        <v>41</v>
+      </c>
+      <c r="B42" s="33">
+        <v>12</v>
+      </c>
+      <c r="C42" s="34" t="s">
+        <v>1046</v>
+      </c>
+      <c r="D42" s="35" t="s">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="23.25" x14ac:dyDescent="0.65">
+      <c r="A43" s="32">
+        <v>42</v>
+      </c>
+      <c r="B43" s="33">
+        <v>12</v>
+      </c>
+      <c r="C43" s="34" t="s">
+        <v>1048</v>
+      </c>
+      <c r="D43" s="35" t="s">
+        <v>1049</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>